<commit_message>
updated edi regular files
</commit_message>
<xml_diff>
--- a/edi_matlab/dinamicadados.xlsx
+++ b/edi_matlab/dinamicadados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Albatroz\Programa EDI\Dinâmica Monoplano\decolagem2022-main\edi_matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuodr\Documents\programaceira\decolagem2022\edi_matlab_bruno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82DE2EB-C5A0-4864-9706-FC70C5AEB2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21C4918-9DE5-4848-B2A0-B64C171DE811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1080" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle" sheetId="1" r:id="rId1"/>
@@ -847,7 +847,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="176">
   <si>
     <t>Variável</t>
   </si>
@@ -1245,9 +1245,6 @@
     <t>Diâmetro</t>
   </si>
   <si>
-    <t>To Corrigida OS 6.1</t>
-  </si>
-  <si>
     <t>N°</t>
   </si>
   <si>
@@ -1359,10 +1356,25 @@
     <t>Coeficiente de atrito da pista (adimensional)</t>
   </si>
   <si>
-    <t>CLmaxw</t>
-  </si>
-  <si>
     <t>21x6.3</t>
+  </si>
+  <si>
+    <t>To Corrigida</t>
+  </si>
+  <si>
+    <t>Sd</t>
+  </si>
+  <si>
+    <t>Distância da pista (m)</t>
+  </si>
+  <si>
+    <t>z_inicial</t>
+  </si>
+  <si>
+    <t>Altura inicial do CG do avião (m)</t>
+  </si>
+  <si>
+    <t>CLmax</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1453,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1538,14 +1550,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1723,33 +1729,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1850,7 +1834,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1896,16 +1879,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2903,16 +2881,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>31115</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>335915</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3693,7 +3671,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3703,101 +3681,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="41">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="41" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="54">
         <v>17</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="42">
         <v>15</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="43">
-        <v>0</v>
-      </c>
-      <c r="C5" s="42" t="s">
+      <c r="B5" s="42">
+        <v>0</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="41">
+        <v>15.3</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="41">
+        <v>0</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="42">
-        <v>0</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="42">
-        <v>0</v>
-      </c>
-      <c r="C8" s="42" t="s">
+      <c r="B8" s="41">
+        <v>0</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="41">
         <v>1</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="41" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3808,10 +3786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780516B4-2B26-4515-B1EB-EE0E9A20E5B7}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3821,276 +3799,298 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="41">
         <v>1.0860000000000001</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="41" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>9.81</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="49">
+      <c r="I3" s="48">
         <v>1000</v>
       </c>
-      <c r="J3" s="50">
-        <f t="shared" ref="J3" si="0">1.255*(1-(0.0065*I3/288.15))^(9.8061/(0.0065*287.05307))</f>
+      <c r="J3" s="49">
+        <f>1.255*(1-(0.0065*I3/288.15))^(9.8061/(0.0065*287.05307))</f>
         <v>1.1131837599499996</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="41">
         <v>0.77</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="41" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="41">
         <v>1.8919999999999999</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="41">
         <v>0.43017</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="41">
         <v>0.9</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="48">
-        <v>0</v>
-      </c>
-      <c r="C8" s="42" t="s">
+      <c r="B8" s="47">
+        <v>0</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="41" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="48">
-        <v>0.17449999999999999</v>
-      </c>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="47">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C9" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="48">
-        <v>0</v>
-      </c>
-      <c r="C10" s="42" t="s">
+      <c r="B10" s="47">
+        <v>0</v>
+      </c>
+      <c r="C10" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="41">
         <v>0.27400000000000002</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="42">
-        <v>0.1285</v>
-      </c>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="41">
+        <v>0</v>
+      </c>
+      <c r="C12" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="47">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="46">
+        <v>0</v>
+      </c>
+      <c r="C13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="46">
         <v>0.39190000000000003</v>
       </c>
-      <c r="C14" s="42">
-        <v>0</v>
-      </c>
-      <c r="D14" s="42">
-        <v>0</v>
-      </c>
-      <c r="F14" s="42" t="s">
+      <c r="C14" s="41">
+        <v>0</v>
+      </c>
+      <c r="D14" s="41">
+        <v>0</v>
+      </c>
+      <c r="F14" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="41" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42">
-        <v>0</v>
-      </c>
-      <c r="C15" s="42">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41">
+        <v>0</v>
+      </c>
+      <c r="C15" s="41">
         <v>0.66600000000000004</v>
       </c>
-      <c r="D15" s="42">
-        <v>0</v>
-      </c>
-      <c r="F15" s="42" t="s">
+      <c r="D15" s="41">
+        <v>0</v>
+      </c>
+      <c r="F15" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="42" t="s">
+      <c r="H15" s="41" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42">
-        <v>0</v>
-      </c>
-      <c r="C16" s="42">
-        <v>0</v>
-      </c>
-      <c r="D16" s="42">
+      <c r="A16" s="41"/>
+      <c r="B16" s="41">
+        <v>0</v>
+      </c>
+      <c r="C16" s="41">
+        <v>0</v>
+      </c>
+      <c r="D16" s="41">
         <v>0.98580000000000001</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="41" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="41">
+        <v>4.53E-2</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="B17" s="42">
-        <v>4.53E-2</v>
-      </c>
-      <c r="C17" s="42" t="s">
+      <c r="B18" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="C18" s="41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="C18" s="42" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="B19" s="41">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="42">
-        <v>0.05</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>169</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="57">
+        <v>58</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="57">
+        <v>0</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4102,8 +4102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7FD063-05B3-470D-AA7D-6BE4832597D6}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4113,19 +4113,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="39"/>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>57</v>
       </c>
       <c r="D1" s="39"/>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>58</v>
       </c>
       <c r="F1" s="39"/>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="40" t="s">
         <v>59</v>
       </c>
       <c r="H1" s="39"/>
@@ -4135,122 +4135,122 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="42">
-        <v>0.77</v>
-      </c>
-      <c r="C2" s="41" t="s">
+      <c r="B2" s="41">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="41">
         <v>0.19070000000000001</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="42">
-        <v>3.2599999999999997E-2</v>
-      </c>
-      <c r="G2" s="41" t="s">
+      <c r="F2" s="41">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G2" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="41">
         <v>4000</v>
       </c>
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
-      <c r="L2" s="51">
-        <v>0</v>
-      </c>
-      <c r="M2" s="52">
+      <c r="L2" s="50">
+        <v>0</v>
+      </c>
+      <c r="M2" s="51">
         <v>3.0599999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>7.0199999999999999E-2</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="41">
         <v>6.4580960000000007E-2</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="42">
+      <c r="H3" s="41">
         <v>5100</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
-      <c r="L3" s="51">
+      <c r="L3" s="50">
         <v>1</v>
       </c>
-      <c r="M3" s="52">
+      <c r="M3" s="51">
         <v>0.04</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="41">
         <v>0.95</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <v>-0.54151700000000003</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="42">
-        <v>0</v>
-      </c>
-      <c r="G4" s="41" t="s">
+      <c r="F4" s="41">
+        <v>0</v>
+      </c>
+      <c r="G4" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="41">
         <v>35</v>
       </c>
       <c r="I4" s="39"/>
       <c r="J4" s="39"/>
-      <c r="L4" s="51">
+      <c r="L4" s="50">
         <v>2</v>
       </c>
-      <c r="M4" s="52">
+      <c r="M4" s="51">
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="41">
         <v>-0.245</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="41">
         <v>0</v>
       </c>
       <c r="E5" s="39"/>
@@ -4259,84 +4259,84 @@
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
-      <c r="L5" s="51">
+      <c r="L5" s="50">
         <v>3</v>
       </c>
-      <c r="M5" s="52">
+      <c r="M5" s="51">
         <v>6.93E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="41">
         <v>-10</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="41">
         <v>-20</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="41">
         <v>-22</v>
       </c>
       <c r="G6" s="39"/>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39"/>
-      <c r="L6" s="51">
+      <c r="L6" s="50">
         <v>4</v>
       </c>
-      <c r="M6" s="52">
+      <c r="M6" s="51">
         <v>8.7099999999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="41">
         <v>15</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="41">
         <v>22</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="41">
         <v>22</v>
       </c>
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
-      <c r="L7" s="51">
+      <c r="L7" s="50">
         <v>5</v>
       </c>
-      <c r="M7" s="52">
+      <c r="M7" s="51">
         <v>0.10440000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="41">
         <v>2</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="41">
         <v>0</v>
       </c>
       <c r="E8" s="39"/>
@@ -4345,24 +4345,24 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
-      <c r="L8" s="51">
+      <c r="L8" s="50">
         <v>6</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="51">
         <v>0.1203</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="41">
         <v>0.70579999999999998</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="41">
         <v>0.55000000000000004</v>
       </c>
       <c r="E9" s="39"/>
@@ -4371,18 +4371,18 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
-      <c r="L9" s="51">
+      <c r="L9" s="50">
         <v>7</v>
       </c>
-      <c r="M9" s="52">
+      <c r="M9" s="51">
         <v>0.1351</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="41">
         <v>7.4312341000000002</v>
       </c>
       <c r="C10" s="39"/>
@@ -4393,79 +4393,79 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
-      <c r="L10" s="51">
+      <c r="L10" s="50">
         <v>8</v>
       </c>
-      <c r="M10" s="52">
+      <c r="M10" s="51">
         <v>0.1502</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="46">
         <v>1E-4</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="47">
-        <v>1E-4</v>
+      <c r="D11" s="46">
+        <v>0</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
-      <c r="H11" s="46"/>
-      <c r="L11" s="51">
+      <c r="H11" s="45"/>
+      <c r="L11" s="50">
         <v>9</v>
       </c>
-      <c r="M11" s="52">
+      <c r="M11" s="51">
         <v>0.1658</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="46">
         <v>1.46E-2</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="47">
-        <v>1.46E-2</v>
+      <c r="D12" s="46">
+        <v>0</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
-      <c r="L12" s="51">
+      <c r="L12" s="50">
         <v>10</v>
       </c>
-      <c r="M12" s="52">
+      <c r="M12" s="51">
         <v>0.18190000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="46">
         <v>2.69E-2</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="47">
-        <v>2.69E-2</v>
+      <c r="D13" s="46">
+        <v>0</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="46">
         <v>0.28299999999999997</v>
       </c>
       <c r="C14" s="39"/>
@@ -4474,11 +4474,11 @@
       <c r="F14" s="39"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="42">
-        <v>2.4824000000000002</v>
+      <c r="A15" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="41">
+        <v>2.5</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -4495,46 +4495,49 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="39"/>
-      <c r="B17" s="47">
-        <v>1E-4</v>
-      </c>
+      <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="47">
+      <c r="B18" s="46">
+        <v>0.68910000000000005</v>
+      </c>
+      <c r="D18">
+        <v>0.45090000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="46">
+        <v>0.41170000000000001</v>
+      </c>
+      <c r="D19">
+        <v>9.7299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="46">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="D20">
+        <v>-6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="46">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="46">
         <v>1.46E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="47">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="46">
         <v>2.69E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="47">
-        <v>0.68910000000000005</v>
-      </c>
-      <c r="D23" s="47">
-        <v>0.37819999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="47">
-        <v>0.41170000000000001</v>
-      </c>
-      <c r="D24" s="47">
-        <v>0.43059999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="47">
-        <v>2.0199999999999999E-2</v>
-      </c>
-      <c r="D25" s="47">
-        <v>1.9900000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4547,339 +4550,1194 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A113401-D5F9-4F05-A1A5-75FFBCA62A3E}">
-  <dimension ref="A1:AS89"/>
+  <dimension ref="A1:BC104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="56">
-        <v>-0.15284</v>
-      </c>
-      <c r="C2" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="39"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>90</v>
       </c>
       <c r="B3" s="56">
-        <v>1.197E-2</v>
-      </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="57">
-        <v>6.5827999999999998E-2</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="57"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="B4" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="57">
-        <v>0</v>
-      </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="B5" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="57">
-        <v>-0.37574000000000002</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="B6" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="57">
-        <v>-5.8846000000000002E-2</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="B7" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="57">
-        <v>8.9717420000000008</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="B8" s="56">
+        <v>7.4755370000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="57">
-        <v>-12.693244</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="B9" s="56">
+        <v>-12.895921</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="57">
-        <v>0</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="B10" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="57">
-        <v>0.26989299999999999</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="B11" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="59">
-        <v>-3.6903999999999999E-2</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="57">
-        <v>-0.120379</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
+      <c r="B12" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="58">
-        <v>0</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="B13" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="58">
-        <v>-0.18941984707025014</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="B14" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="58">
-        <v>0</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" s="58">
+      <c r="B15" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="56">
         <v>0.67482969110508362</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="58">
-        <v>-1.6843813261255942</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="B17" s="56">
+        <v>-1.6776204241430506</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="58">
-        <v>2.4121523175007702E-2</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="B18" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="58">
-        <v>0</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="42" t="s">
+      <c r="B19" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="58">
-        <v>-1.4495832216809799E-2</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="39"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="39"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="65" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM65" s="40"/>
-    </row>
-    <row r="66" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM66" s="40"/>
-    </row>
-    <row r="67" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM67" s="40"/>
-    </row>
-    <row r="68" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM68" s="40"/>
-    </row>
-    <row r="69" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM69" s="40"/>
-      <c r="AR69" s="40"/>
-    </row>
-    <row r="70" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM70" s="40"/>
-    </row>
-    <row r="71" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM71" s="40"/>
-      <c r="AQ71" s="40"/>
-    </row>
-    <row r="72" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM72" s="40"/>
-    </row>
-    <row r="73" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM73" s="40"/>
-      <c r="AP73" s="40"/>
-    </row>
-    <row r="74" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM74" s="40"/>
-      <c r="AO74" s="40"/>
-    </row>
-    <row r="75" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM75" s="40"/>
-    </row>
-    <row r="76" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM76" s="40"/>
-      <c r="AN76" s="40"/>
-    </row>
-    <row r="77" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM77" s="40"/>
-      <c r="AN77" s="40"/>
-    </row>
-    <row r="78" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM78" s="40"/>
-    </row>
-    <row r="79" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM79" s="40"/>
-      <c r="AO79" s="40"/>
-    </row>
-    <row r="80" spans="39:44" x14ac:dyDescent="0.3">
-      <c r="AM80" s="40"/>
-      <c r="AP80" s="40"/>
-    </row>
-    <row r="81" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM81" s="40"/>
-      <c r="AQ81" s="40"/>
-    </row>
-    <row r="82" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM82" s="40"/>
-      <c r="AR82" s="40"/>
-    </row>
-    <row r="83" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM83" s="40"/>
-      <c r="AQ83" s="40"/>
-    </row>
-    <row r="84" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM84" s="40"/>
-    </row>
-    <row r="85" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM85" s="40"/>
-      <c r="AR85" s="40"/>
-    </row>
-    <row r="86" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM86" s="40"/>
-      <c r="AS86" s="40"/>
-    </row>
-    <row r="87" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM87" s="40"/>
-      <c r="AS87" s="40"/>
-    </row>
-    <row r="88" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM88" s="40"/>
-      <c r="AS88" s="40"/>
-    </row>
-    <row r="89" spans="39:45" x14ac:dyDescent="0.3">
-      <c r="AM89" s="40"/>
+    </row>
+    <row r="58" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK58" s="55"/>
+      <c r="AL58" s="55"/>
+      <c r="AM58" s="55"/>
+      <c r="AN58" s="55"/>
+      <c r="AO58" s="55"/>
+      <c r="AP58" s="55"/>
+      <c r="AQ58" s="55"/>
+      <c r="AR58" s="55"/>
+      <c r="AS58" s="55"/>
+      <c r="AT58" s="55"/>
+      <c r="AU58" s="55"/>
+      <c r="AV58" s="55"/>
+      <c r="AW58" s="55"/>
+      <c r="AX58" s="55"/>
+      <c r="AY58" s="55"/>
+      <c r="AZ58" s="55"/>
+      <c r="BA58" s="55"/>
+      <c r="BB58" s="55"/>
+      <c r="BC58" s="55"/>
+    </row>
+    <row r="59" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK59" s="55"/>
+      <c r="AL59" s="55"/>
+      <c r="AM59" s="55"/>
+      <c r="AN59" s="55"/>
+      <c r="AO59" s="55"/>
+      <c r="AP59" s="55"/>
+      <c r="AQ59" s="55"/>
+      <c r="AR59" s="55"/>
+      <c r="AS59" s="55"/>
+      <c r="AT59" s="55"/>
+      <c r="AU59" s="55"/>
+      <c r="AV59" s="55"/>
+      <c r="AW59" s="55"/>
+      <c r="AX59" s="55"/>
+      <c r="AY59" s="55"/>
+      <c r="AZ59" s="55"/>
+      <c r="BA59" s="55"/>
+      <c r="BB59" s="55"/>
+      <c r="BC59" s="55"/>
+    </row>
+    <row r="60" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK60" s="55"/>
+      <c r="AL60" s="55"/>
+      <c r="AM60" s="55"/>
+      <c r="AN60" s="55"/>
+      <c r="AO60" s="55"/>
+      <c r="AP60" s="55"/>
+      <c r="AQ60" s="55"/>
+      <c r="AR60" s="55"/>
+      <c r="AS60" s="55"/>
+      <c r="AT60" s="55"/>
+      <c r="AU60" s="55"/>
+      <c r="AV60" s="55"/>
+      <c r="AW60" s="55"/>
+      <c r="AX60" s="55"/>
+      <c r="AY60" s="55"/>
+      <c r="AZ60" s="55"/>
+      <c r="BA60" s="55"/>
+      <c r="BB60" s="55"/>
+      <c r="BC60" s="55"/>
+    </row>
+    <row r="61" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK61" s="55"/>
+      <c r="AL61" s="55"/>
+      <c r="AM61" s="55"/>
+      <c r="AN61" s="55"/>
+      <c r="AO61" s="55"/>
+      <c r="AP61" s="55"/>
+      <c r="AQ61" s="55"/>
+      <c r="AR61" s="55"/>
+      <c r="AS61" s="55"/>
+      <c r="AT61" s="55"/>
+      <c r="AU61" s="55"/>
+      <c r="AV61" s="55"/>
+      <c r="AW61" s="55"/>
+      <c r="AX61" s="55"/>
+      <c r="AY61" s="55"/>
+      <c r="AZ61" s="55"/>
+      <c r="BA61" s="55"/>
+      <c r="BB61" s="55"/>
+      <c r="BC61" s="55"/>
+    </row>
+    <row r="62" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK62" s="55"/>
+      <c r="AL62" s="55"/>
+      <c r="AM62" s="55"/>
+      <c r="AN62" s="55"/>
+      <c r="AO62" s="55"/>
+      <c r="AP62" s="55"/>
+      <c r="AQ62" s="55"/>
+      <c r="AR62" s="55"/>
+      <c r="AS62" s="55"/>
+      <c r="AT62" s="55"/>
+      <c r="AU62" s="55"/>
+      <c r="AV62" s="55"/>
+      <c r="AW62" s="55"/>
+      <c r="AX62" s="55"/>
+      <c r="AY62" s="55"/>
+      <c r="AZ62" s="55"/>
+      <c r="BA62" s="55"/>
+      <c r="BB62" s="55"/>
+      <c r="BC62" s="55"/>
+    </row>
+    <row r="63" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK63" s="55"/>
+      <c r="AL63" s="55"/>
+      <c r="AM63" s="55"/>
+      <c r="AN63" s="55"/>
+      <c r="AO63" s="55"/>
+      <c r="AP63" s="55"/>
+      <c r="AQ63" s="55"/>
+      <c r="AR63" s="55"/>
+      <c r="AS63" s="55"/>
+      <c r="AT63" s="55"/>
+      <c r="AU63" s="55"/>
+      <c r="AV63" s="55"/>
+      <c r="AW63" s="55"/>
+      <c r="AX63" s="55"/>
+      <c r="AY63" s="55"/>
+      <c r="AZ63" s="55"/>
+      <c r="BA63" s="55"/>
+      <c r="BB63" s="55"/>
+      <c r="BC63" s="55"/>
+    </row>
+    <row r="64" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK64" s="55"/>
+      <c r="AL64" s="55"/>
+      <c r="AM64" s="55"/>
+      <c r="AN64" s="55"/>
+      <c r="AO64" s="55"/>
+      <c r="AP64" s="55"/>
+      <c r="AQ64" s="55"/>
+      <c r="AR64" s="55"/>
+      <c r="AS64" s="55"/>
+      <c r="AT64" s="55"/>
+      <c r="AU64" s="55"/>
+      <c r="AV64" s="55"/>
+      <c r="AW64" s="55"/>
+      <c r="AX64" s="55"/>
+      <c r="AY64" s="55"/>
+      <c r="AZ64" s="55"/>
+      <c r="BA64" s="55"/>
+      <c r="BB64" s="55"/>
+      <c r="BC64" s="55"/>
+    </row>
+    <row r="65" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK65" s="55"/>
+      <c r="AL65" s="55"/>
+      <c r="AM65" s="55"/>
+      <c r="AN65" s="55"/>
+      <c r="AO65" s="55"/>
+      <c r="AP65" s="55"/>
+      <c r="AQ65" s="55"/>
+      <c r="AR65" s="55"/>
+      <c r="AS65" s="55"/>
+      <c r="AT65" s="55"/>
+      <c r="AU65" s="55"/>
+      <c r="AV65" s="55"/>
+      <c r="AW65" s="55"/>
+      <c r="AX65" s="55"/>
+      <c r="AY65" s="55"/>
+      <c r="AZ65" s="55"/>
+      <c r="BA65" s="55"/>
+      <c r="BB65" s="55"/>
+      <c r="BC65" s="55"/>
+    </row>
+    <row r="66" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK66" s="55"/>
+      <c r="AL66" s="55"/>
+      <c r="AM66" s="55"/>
+      <c r="AN66" s="55"/>
+      <c r="AO66" s="55"/>
+      <c r="AP66" s="55"/>
+      <c r="AQ66" s="55"/>
+      <c r="AR66" s="55"/>
+      <c r="AS66" s="55"/>
+      <c r="AT66" s="55"/>
+      <c r="AU66" s="55"/>
+      <c r="AV66" s="55"/>
+      <c r="AW66" s="55"/>
+      <c r="AX66" s="55"/>
+      <c r="AY66" s="55"/>
+      <c r="AZ66" s="55"/>
+      <c r="BA66" s="55"/>
+      <c r="BB66" s="55"/>
+      <c r="BC66" s="55"/>
+    </row>
+    <row r="67" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK67" s="55"/>
+      <c r="AL67" s="55"/>
+      <c r="AM67" s="55"/>
+      <c r="AN67" s="55"/>
+      <c r="AO67" s="55"/>
+      <c r="AP67" s="55"/>
+      <c r="AQ67" s="55"/>
+      <c r="AR67" s="55"/>
+      <c r="AS67" s="55"/>
+      <c r="AT67" s="55"/>
+      <c r="AU67" s="55"/>
+      <c r="AV67" s="55"/>
+      <c r="AW67" s="55"/>
+      <c r="AX67" s="55"/>
+      <c r="AY67" s="55"/>
+      <c r="AZ67" s="55"/>
+      <c r="BA67" s="55"/>
+      <c r="BB67" s="55"/>
+      <c r="BC67" s="55"/>
+    </row>
+    <row r="68" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK68" s="55"/>
+      <c r="AL68" s="55"/>
+      <c r="AM68" s="55"/>
+      <c r="AN68" s="55"/>
+      <c r="AO68" s="55"/>
+      <c r="AP68" s="55"/>
+      <c r="AQ68" s="55"/>
+      <c r="AR68" s="55"/>
+      <c r="AS68" s="55"/>
+      <c r="AT68" s="55"/>
+      <c r="AU68" s="55"/>
+      <c r="AV68" s="55"/>
+      <c r="AW68" s="55"/>
+      <c r="AX68" s="55"/>
+      <c r="AY68" s="55"/>
+      <c r="AZ68" s="55"/>
+      <c r="BA68" s="55"/>
+      <c r="BB68" s="55"/>
+      <c r="BC68" s="55"/>
+    </row>
+    <row r="69" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK69" s="55"/>
+      <c r="AL69" s="55"/>
+      <c r="AM69" s="55"/>
+      <c r="AN69" s="55"/>
+      <c r="AO69" s="55"/>
+      <c r="AP69" s="55"/>
+      <c r="AQ69" s="55"/>
+      <c r="AR69" s="55"/>
+      <c r="AS69" s="55"/>
+      <c r="AT69" s="55"/>
+      <c r="AU69" s="55"/>
+      <c r="AV69" s="55"/>
+      <c r="AW69" s="55"/>
+      <c r="AX69" s="55"/>
+      <c r="AY69" s="55"/>
+      <c r="AZ69" s="55"/>
+      <c r="BA69" s="55"/>
+      <c r="BB69" s="55"/>
+      <c r="BC69" s="55"/>
+    </row>
+    <row r="70" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK70" s="55"/>
+      <c r="AL70" s="55"/>
+      <c r="AM70" s="55"/>
+      <c r="AN70" s="55"/>
+      <c r="AO70" s="55"/>
+      <c r="AP70" s="55"/>
+      <c r="AQ70" s="55"/>
+      <c r="AR70" s="55"/>
+      <c r="AS70" s="55"/>
+      <c r="AT70" s="55"/>
+      <c r="AU70" s="55"/>
+      <c r="AV70" s="55"/>
+      <c r="AW70" s="55"/>
+      <c r="AX70" s="55"/>
+      <c r="AY70" s="55"/>
+      <c r="AZ70" s="55"/>
+      <c r="BA70" s="55"/>
+      <c r="BB70" s="55"/>
+      <c r="BC70" s="55"/>
+    </row>
+    <row r="71" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK71" s="55"/>
+      <c r="AL71" s="55"/>
+      <c r="AM71" s="55"/>
+      <c r="AN71" s="55"/>
+      <c r="AO71" s="55"/>
+      <c r="AP71" s="55"/>
+      <c r="AQ71" s="55"/>
+      <c r="AR71" s="55"/>
+      <c r="AS71" s="55"/>
+      <c r="AT71" s="55"/>
+      <c r="AU71" s="55"/>
+      <c r="AV71" s="55"/>
+      <c r="AW71" s="55"/>
+      <c r="AX71" s="55"/>
+      <c r="AY71" s="55"/>
+      <c r="AZ71" s="55"/>
+      <c r="BA71" s="55"/>
+      <c r="BB71" s="55"/>
+      <c r="BC71" s="55"/>
+    </row>
+    <row r="72" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK72" s="55"/>
+      <c r="AL72" s="55"/>
+      <c r="AM72" s="55"/>
+      <c r="AN72" s="55"/>
+      <c r="AO72" s="55"/>
+      <c r="AP72" s="55"/>
+      <c r="AQ72" s="55"/>
+      <c r="AR72" s="55"/>
+      <c r="AS72" s="55"/>
+      <c r="AT72" s="55"/>
+      <c r="AU72" s="55"/>
+      <c r="AV72" s="55"/>
+      <c r="AW72" s="55"/>
+      <c r="AX72" s="55"/>
+      <c r="AY72" s="55"/>
+      <c r="AZ72" s="55"/>
+      <c r="BA72" s="55"/>
+      <c r="BB72" s="55"/>
+      <c r="BC72" s="55"/>
+    </row>
+    <row r="73" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK73" s="55"/>
+      <c r="AL73" s="55"/>
+      <c r="AM73" s="55"/>
+      <c r="AN73" s="55"/>
+      <c r="AO73" s="55"/>
+      <c r="AP73" s="55"/>
+      <c r="AQ73" s="55"/>
+      <c r="AR73" s="55"/>
+      <c r="AS73" s="55"/>
+      <c r="AT73" s="55"/>
+      <c r="AU73" s="55"/>
+      <c r="AV73" s="55"/>
+      <c r="AW73" s="55"/>
+      <c r="AX73" s="55"/>
+      <c r="AY73" s="55"/>
+      <c r="AZ73" s="55"/>
+      <c r="BA73" s="55"/>
+      <c r="BB73" s="55"/>
+      <c r="BC73" s="55"/>
+    </row>
+    <row r="74" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK74" s="55"/>
+      <c r="AL74" s="55"/>
+      <c r="AM74" s="55"/>
+      <c r="AN74" s="55"/>
+      <c r="AO74" s="55"/>
+      <c r="AP74" s="55"/>
+      <c r="AQ74" s="55"/>
+      <c r="AR74" s="55"/>
+      <c r="AS74" s="55"/>
+      <c r="AT74" s="55"/>
+      <c r="AU74" s="55"/>
+      <c r="AV74" s="55"/>
+      <c r="AW74" s="55"/>
+      <c r="AX74" s="55"/>
+      <c r="AY74" s="55"/>
+      <c r="AZ74" s="55"/>
+      <c r="BA74" s="55"/>
+      <c r="BB74" s="55"/>
+      <c r="BC74" s="55"/>
+    </row>
+    <row r="75" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK75" s="55"/>
+      <c r="AL75" s="55"/>
+      <c r="AM75" s="55"/>
+      <c r="AN75" s="55"/>
+      <c r="AO75" s="55"/>
+      <c r="AP75" s="55"/>
+      <c r="AQ75" s="55"/>
+      <c r="AR75" s="55"/>
+      <c r="AS75" s="55"/>
+      <c r="AT75" s="55"/>
+      <c r="AU75" s="55"/>
+      <c r="AV75" s="55"/>
+      <c r="AW75" s="55"/>
+      <c r="AX75" s="55"/>
+      <c r="AY75" s="55"/>
+      <c r="AZ75" s="55"/>
+      <c r="BA75" s="55"/>
+      <c r="BB75" s="55"/>
+      <c r="BC75" s="55"/>
+    </row>
+    <row r="76" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK76" s="55"/>
+      <c r="AL76" s="55"/>
+      <c r="AM76" s="55"/>
+      <c r="AN76" s="55"/>
+      <c r="AO76" s="55"/>
+      <c r="AP76" s="55"/>
+      <c r="AQ76" s="55"/>
+      <c r="AR76" s="55"/>
+      <c r="AS76" s="55"/>
+      <c r="AT76" s="55"/>
+      <c r="AU76" s="55"/>
+      <c r="AV76" s="55"/>
+      <c r="AW76" s="55"/>
+      <c r="AX76" s="55"/>
+      <c r="AY76" s="55"/>
+      <c r="AZ76" s="55"/>
+      <c r="BA76" s="55"/>
+      <c r="BB76" s="55"/>
+      <c r="BC76" s="55"/>
+    </row>
+    <row r="77" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK77" s="55"/>
+      <c r="AL77" s="55"/>
+      <c r="AM77" s="55"/>
+      <c r="AN77" s="55"/>
+      <c r="AO77" s="55"/>
+      <c r="AP77" s="55"/>
+      <c r="AQ77" s="55"/>
+      <c r="AR77" s="55"/>
+      <c r="AS77" s="55"/>
+      <c r="AT77" s="55"/>
+      <c r="AU77" s="55"/>
+      <c r="AV77" s="55"/>
+      <c r="AW77" s="55"/>
+      <c r="AX77" s="55"/>
+      <c r="AY77" s="55"/>
+      <c r="AZ77" s="55"/>
+      <c r="BA77" s="55"/>
+      <c r="BB77" s="55"/>
+      <c r="BC77" s="55"/>
+    </row>
+    <row r="78" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK78" s="55"/>
+      <c r="AL78" s="55"/>
+      <c r="AM78" s="55"/>
+      <c r="AN78" s="55"/>
+      <c r="AO78" s="55"/>
+      <c r="AP78" s="55"/>
+      <c r="AQ78" s="55"/>
+      <c r="AR78" s="55"/>
+      <c r="AS78" s="55"/>
+      <c r="AT78" s="55"/>
+      <c r="AU78" s="55"/>
+      <c r="AV78" s="55"/>
+      <c r="AW78" s="55"/>
+      <c r="AX78" s="55"/>
+      <c r="AY78" s="55"/>
+      <c r="AZ78" s="55"/>
+      <c r="BA78" s="55"/>
+      <c r="BB78" s="55"/>
+      <c r="BC78" s="55"/>
+    </row>
+    <row r="79" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK79" s="55"/>
+      <c r="AL79" s="55"/>
+      <c r="AM79" s="55"/>
+      <c r="AN79" s="55"/>
+      <c r="AO79" s="55"/>
+      <c r="AP79" s="55"/>
+      <c r="AQ79" s="55"/>
+      <c r="AR79" s="55"/>
+      <c r="AS79" s="55"/>
+      <c r="AT79" s="55"/>
+      <c r="AU79" s="55"/>
+      <c r="AV79" s="55"/>
+      <c r="AW79" s="55"/>
+      <c r="AX79" s="55"/>
+      <c r="AY79" s="55"/>
+      <c r="AZ79" s="55"/>
+      <c r="BA79" s="55"/>
+      <c r="BB79" s="55"/>
+      <c r="BC79" s="55"/>
+    </row>
+    <row r="80" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK80" s="55"/>
+      <c r="AL80" s="55"/>
+      <c r="AM80" s="55"/>
+      <c r="AN80" s="55"/>
+      <c r="AO80" s="55"/>
+      <c r="AP80" s="55"/>
+      <c r="AQ80" s="55"/>
+      <c r="AR80" s="55"/>
+      <c r="AS80" s="55"/>
+      <c r="AT80" s="55"/>
+      <c r="AU80" s="55"/>
+      <c r="AV80" s="55"/>
+      <c r="AW80" s="55"/>
+      <c r="AX80" s="55"/>
+      <c r="AY80" s="55"/>
+      <c r="AZ80" s="55"/>
+      <c r="BA80" s="55"/>
+      <c r="BB80" s="55"/>
+      <c r="BC80" s="55"/>
+    </row>
+    <row r="81" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK81" s="55"/>
+      <c r="AL81" s="55"/>
+      <c r="AM81" s="55"/>
+      <c r="AN81" s="55"/>
+      <c r="AO81" s="55"/>
+      <c r="AP81" s="55"/>
+      <c r="AQ81" s="55"/>
+      <c r="AR81" s="55"/>
+      <c r="AS81" s="55"/>
+      <c r="AT81" s="55"/>
+      <c r="AU81" s="55"/>
+      <c r="AV81" s="55"/>
+      <c r="AW81" s="55"/>
+      <c r="AX81" s="55"/>
+      <c r="AY81" s="55"/>
+      <c r="AZ81" s="55"/>
+      <c r="BA81" s="55"/>
+      <c r="BB81" s="55"/>
+      <c r="BC81" s="55"/>
+    </row>
+    <row r="82" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK82" s="55"/>
+      <c r="AL82" s="55"/>
+      <c r="AM82" s="55"/>
+      <c r="AN82" s="55"/>
+      <c r="AO82" s="55"/>
+      <c r="AP82" s="55"/>
+      <c r="AQ82" s="55"/>
+      <c r="AR82" s="55"/>
+      <c r="AS82" s="55"/>
+      <c r="AT82" s="55"/>
+      <c r="AU82" s="55"/>
+      <c r="AV82" s="55"/>
+      <c r="AW82" s="55"/>
+      <c r="AX82" s="55"/>
+      <c r="AY82" s="55"/>
+      <c r="AZ82" s="55"/>
+      <c r="BA82" s="55"/>
+      <c r="BB82" s="55"/>
+      <c r="BC82" s="55"/>
+    </row>
+    <row r="83" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK83" s="55"/>
+      <c r="AL83" s="55"/>
+      <c r="AM83" s="55"/>
+      <c r="AN83" s="55"/>
+      <c r="AO83" s="55"/>
+      <c r="AP83" s="55"/>
+      <c r="AQ83" s="55"/>
+      <c r="AR83" s="55"/>
+      <c r="AS83" s="55"/>
+      <c r="AT83" s="55"/>
+      <c r="AU83" s="55"/>
+      <c r="AV83" s="55"/>
+      <c r="AW83" s="55"/>
+      <c r="AX83" s="55"/>
+      <c r="AY83" s="55"/>
+      <c r="AZ83" s="55"/>
+      <c r="BA83" s="55"/>
+      <c r="BB83" s="55"/>
+      <c r="BC83" s="55"/>
+    </row>
+    <row r="84" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK84" s="55"/>
+      <c r="AL84" s="55"/>
+      <c r="AM84" s="55"/>
+      <c r="AN84" s="55"/>
+      <c r="AO84" s="55"/>
+      <c r="AP84" s="55"/>
+      <c r="AQ84" s="55"/>
+      <c r="AR84" s="55"/>
+      <c r="AS84" s="55"/>
+      <c r="AT84" s="55"/>
+      <c r="AU84" s="55"/>
+      <c r="AV84" s="55"/>
+      <c r="AW84" s="55"/>
+      <c r="AX84" s="55"/>
+      <c r="AY84" s="55"/>
+      <c r="AZ84" s="55"/>
+      <c r="BA84" s="55"/>
+      <c r="BB84" s="55"/>
+      <c r="BC84" s="55"/>
+    </row>
+    <row r="85" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK85" s="55"/>
+      <c r="AL85" s="55"/>
+      <c r="AM85" s="55"/>
+      <c r="AN85" s="55"/>
+      <c r="AO85" s="55"/>
+      <c r="AP85" s="55"/>
+      <c r="AQ85" s="55"/>
+      <c r="AR85" s="55"/>
+      <c r="AS85" s="55"/>
+      <c r="AT85" s="55"/>
+      <c r="AU85" s="55"/>
+      <c r="AV85" s="55"/>
+      <c r="AW85" s="55"/>
+      <c r="AX85" s="55"/>
+      <c r="AY85" s="55"/>
+      <c r="AZ85" s="55"/>
+      <c r="BA85" s="55"/>
+      <c r="BB85" s="55"/>
+      <c r="BC85" s="55"/>
+    </row>
+    <row r="86" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK86" s="55"/>
+      <c r="AL86" s="55"/>
+      <c r="AM86" s="55"/>
+      <c r="AN86" s="55"/>
+      <c r="AO86" s="55"/>
+      <c r="AP86" s="55"/>
+      <c r="AQ86" s="55"/>
+      <c r="AR86" s="55"/>
+      <c r="AS86" s="55"/>
+      <c r="AT86" s="55"/>
+      <c r="AU86" s="55"/>
+      <c r="AV86" s="55"/>
+      <c r="AW86" s="55"/>
+      <c r="AX86" s="55"/>
+      <c r="AY86" s="55"/>
+      <c r="AZ86" s="55"/>
+      <c r="BA86" s="55"/>
+      <c r="BB86" s="55"/>
+      <c r="BC86" s="55"/>
+    </row>
+    <row r="87" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK87" s="55"/>
+      <c r="AL87" s="55"/>
+      <c r="AM87" s="55"/>
+      <c r="AN87" s="55"/>
+      <c r="AO87" s="55"/>
+      <c r="AP87" s="55"/>
+      <c r="AQ87" s="55"/>
+      <c r="AR87" s="55"/>
+      <c r="AS87" s="55"/>
+      <c r="AT87" s="55"/>
+      <c r="AU87" s="55"/>
+      <c r="AV87" s="55"/>
+      <c r="AW87" s="55"/>
+      <c r="AX87" s="55"/>
+      <c r="AY87" s="55"/>
+      <c r="AZ87" s="55"/>
+      <c r="BA87" s="55"/>
+      <c r="BB87" s="55"/>
+      <c r="BC87" s="55"/>
+    </row>
+    <row r="88" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK88" s="55"/>
+      <c r="AL88" s="55"/>
+      <c r="AM88" s="55"/>
+      <c r="AN88" s="55"/>
+      <c r="AO88" s="55"/>
+      <c r="AP88" s="55"/>
+      <c r="AQ88" s="55"/>
+      <c r="AR88" s="55"/>
+      <c r="AS88" s="55"/>
+      <c r="AT88" s="55"/>
+      <c r="AU88" s="55"/>
+      <c r="AV88" s="55"/>
+      <c r="AW88" s="55"/>
+      <c r="AX88" s="55"/>
+      <c r="AY88" s="55"/>
+      <c r="AZ88" s="55"/>
+      <c r="BA88" s="55"/>
+      <c r="BB88" s="55"/>
+      <c r="BC88" s="55"/>
+    </row>
+    <row r="89" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK89" s="55"/>
+      <c r="AL89" s="55"/>
+      <c r="AM89" s="55"/>
+      <c r="AN89" s="55"/>
+      <c r="AO89" s="55"/>
+      <c r="AP89" s="55"/>
+      <c r="AQ89" s="55"/>
+      <c r="AR89" s="55"/>
+      <c r="AS89" s="55"/>
+      <c r="AT89" s="55"/>
+      <c r="AU89" s="55"/>
+      <c r="AV89" s="55"/>
+      <c r="AW89" s="55"/>
+      <c r="AX89" s="55"/>
+      <c r="AY89" s="55"/>
+      <c r="AZ89" s="55"/>
+      <c r="BA89" s="55"/>
+      <c r="BB89" s="55"/>
+      <c r="BC89" s="55"/>
+    </row>
+    <row r="90" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK90" s="55"/>
+      <c r="AL90" s="55"/>
+      <c r="AM90" s="55"/>
+      <c r="AN90" s="55"/>
+      <c r="AO90" s="55"/>
+      <c r="AP90" s="55"/>
+      <c r="AQ90" s="55"/>
+      <c r="AR90" s="55"/>
+      <c r="AS90" s="55"/>
+      <c r="AT90" s="55"/>
+      <c r="AU90" s="55"/>
+      <c r="AV90" s="55"/>
+      <c r="AW90" s="55"/>
+      <c r="AX90" s="55"/>
+      <c r="AY90" s="55"/>
+      <c r="AZ90" s="55"/>
+      <c r="BA90" s="55"/>
+      <c r="BB90" s="55"/>
+      <c r="BC90" s="55"/>
+    </row>
+    <row r="91" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK91" s="55"/>
+      <c r="AL91" s="55"/>
+      <c r="AM91" s="55"/>
+      <c r="AN91" s="55"/>
+      <c r="AO91" s="55"/>
+      <c r="AP91" s="55"/>
+      <c r="AQ91" s="55"/>
+      <c r="AR91" s="55"/>
+      <c r="AS91" s="55"/>
+      <c r="AT91" s="55"/>
+      <c r="AU91" s="55"/>
+      <c r="AV91" s="55"/>
+      <c r="AW91" s="55"/>
+      <c r="AX91" s="55"/>
+      <c r="AY91" s="55"/>
+      <c r="AZ91" s="55"/>
+      <c r="BA91" s="55"/>
+      <c r="BB91" s="55"/>
+      <c r="BC91" s="55"/>
+    </row>
+    <row r="92" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK92" s="55"/>
+      <c r="AL92" s="55"/>
+      <c r="AM92" s="55"/>
+      <c r="AN92" s="55"/>
+      <c r="AO92" s="55"/>
+      <c r="AP92" s="55"/>
+      <c r="AQ92" s="55"/>
+      <c r="AR92" s="55"/>
+      <c r="AS92" s="55"/>
+      <c r="AT92" s="55"/>
+      <c r="AU92" s="55"/>
+      <c r="AV92" s="55"/>
+      <c r="AW92" s="55"/>
+      <c r="AX92" s="55"/>
+      <c r="AY92" s="55"/>
+      <c r="AZ92" s="55"/>
+      <c r="BA92" s="55"/>
+      <c r="BB92" s="55"/>
+      <c r="BC92" s="55"/>
+    </row>
+    <row r="93" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK93" s="55"/>
+      <c r="AL93" s="55"/>
+      <c r="AM93" s="55"/>
+      <c r="AN93" s="55"/>
+      <c r="AO93" s="55"/>
+      <c r="AP93" s="55"/>
+      <c r="AQ93" s="55"/>
+      <c r="AR93" s="55"/>
+      <c r="AS93" s="55"/>
+      <c r="AT93" s="55"/>
+      <c r="AU93" s="55"/>
+      <c r="AV93" s="55"/>
+      <c r="AW93" s="55"/>
+      <c r="AX93" s="55"/>
+      <c r="AY93" s="55"/>
+      <c r="AZ93" s="55"/>
+      <c r="BA93" s="55"/>
+      <c r="BB93" s="55"/>
+      <c r="BC93" s="55"/>
+    </row>
+    <row r="94" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK94" s="55"/>
+      <c r="AL94" s="55"/>
+      <c r="AM94" s="55"/>
+      <c r="AN94" s="55"/>
+      <c r="AO94" s="55"/>
+      <c r="AP94" s="55"/>
+      <c r="AQ94" s="55"/>
+      <c r="AR94" s="55"/>
+      <c r="AS94" s="55"/>
+      <c r="AT94" s="55"/>
+      <c r="AU94" s="55"/>
+      <c r="AV94" s="55"/>
+      <c r="AW94" s="55"/>
+      <c r="AX94" s="55"/>
+      <c r="AY94" s="55"/>
+      <c r="AZ94" s="55"/>
+      <c r="BA94" s="55"/>
+      <c r="BB94" s="55"/>
+      <c r="BC94" s="55"/>
+    </row>
+    <row r="95" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK95" s="55"/>
+      <c r="AL95" s="55"/>
+      <c r="AM95" s="55"/>
+      <c r="AN95" s="55"/>
+      <c r="AO95" s="55"/>
+      <c r="AP95" s="55"/>
+      <c r="AQ95" s="55"/>
+      <c r="AR95" s="55"/>
+      <c r="AS95" s="55"/>
+      <c r="AT95" s="55"/>
+      <c r="AU95" s="55"/>
+      <c r="AV95" s="55"/>
+      <c r="AW95" s="55"/>
+      <c r="AX95" s="55"/>
+      <c r="AY95" s="55"/>
+      <c r="AZ95" s="55"/>
+      <c r="BA95" s="55"/>
+      <c r="BB95" s="55"/>
+      <c r="BC95" s="55"/>
+    </row>
+    <row r="96" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK96" s="55"/>
+      <c r="AL96" s="55"/>
+      <c r="AM96" s="55"/>
+      <c r="AN96" s="55"/>
+      <c r="AO96" s="55"/>
+      <c r="AP96" s="55"/>
+      <c r="AQ96" s="55"/>
+      <c r="AR96" s="55"/>
+      <c r="AS96" s="55"/>
+      <c r="AT96" s="55"/>
+      <c r="AU96" s="55"/>
+      <c r="AV96" s="55"/>
+      <c r="AW96" s="55"/>
+      <c r="AX96" s="55"/>
+      <c r="AY96" s="55"/>
+      <c r="AZ96" s="55"/>
+      <c r="BA96" s="55"/>
+      <c r="BB96" s="55"/>
+      <c r="BC96" s="55"/>
+    </row>
+    <row r="97" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK97" s="55"/>
+      <c r="AL97" s="55"/>
+      <c r="AM97" s="55"/>
+      <c r="AN97" s="55"/>
+      <c r="AO97" s="55"/>
+      <c r="AP97" s="55"/>
+      <c r="AQ97" s="55"/>
+      <c r="AR97" s="55"/>
+      <c r="AS97" s="55"/>
+      <c r="AT97" s="55"/>
+      <c r="AU97" s="55"/>
+      <c r="AV97" s="55"/>
+      <c r="AW97" s="55"/>
+      <c r="AX97" s="55"/>
+      <c r="AY97" s="55"/>
+      <c r="AZ97" s="55"/>
+      <c r="BA97" s="55"/>
+      <c r="BB97" s="55"/>
+      <c r="BC97" s="55"/>
+    </row>
+    <row r="98" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK98" s="55"/>
+      <c r="AL98" s="55"/>
+      <c r="AM98" s="55"/>
+      <c r="AN98" s="55"/>
+      <c r="AO98" s="55"/>
+      <c r="AP98" s="55"/>
+      <c r="AQ98" s="55"/>
+      <c r="AR98" s="55"/>
+      <c r="AS98" s="55"/>
+      <c r="AT98" s="55"/>
+      <c r="AU98" s="55"/>
+      <c r="AV98" s="55"/>
+      <c r="AW98" s="55"/>
+      <c r="AX98" s="55"/>
+      <c r="AY98" s="55"/>
+      <c r="AZ98" s="55"/>
+      <c r="BA98" s="55"/>
+      <c r="BB98" s="55"/>
+      <c r="BC98" s="55"/>
+    </row>
+    <row r="99" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK99" s="55"/>
+      <c r="AL99" s="55"/>
+      <c r="AM99" s="55"/>
+      <c r="AN99" s="55"/>
+      <c r="AO99" s="55"/>
+      <c r="AP99" s="55"/>
+      <c r="AQ99" s="55"/>
+      <c r="AR99" s="55"/>
+      <c r="AS99" s="55"/>
+      <c r="AT99" s="55"/>
+      <c r="AU99" s="55"/>
+      <c r="AV99" s="55"/>
+      <c r="AW99" s="55"/>
+      <c r="AX99" s="55"/>
+      <c r="AY99" s="55"/>
+      <c r="AZ99" s="55"/>
+      <c r="BA99" s="55"/>
+      <c r="BB99" s="55"/>
+      <c r="BC99" s="55"/>
+    </row>
+    <row r="100" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK100" s="55"/>
+      <c r="AL100" s="55"/>
+      <c r="AM100" s="55"/>
+      <c r="AN100" s="55"/>
+      <c r="AO100" s="55"/>
+      <c r="AP100" s="55"/>
+      <c r="AQ100" s="55"/>
+      <c r="AR100" s="55"/>
+      <c r="AS100" s="55"/>
+      <c r="AT100" s="55"/>
+      <c r="AU100" s="55"/>
+      <c r="AV100" s="55"/>
+      <c r="AW100" s="55"/>
+      <c r="AX100" s="55"/>
+      <c r="AY100" s="55"/>
+      <c r="AZ100" s="55"/>
+      <c r="BA100" s="55"/>
+      <c r="BB100" s="55"/>
+      <c r="BC100" s="55"/>
+    </row>
+    <row r="101" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK101" s="55"/>
+      <c r="AL101" s="55"/>
+      <c r="AM101" s="55"/>
+      <c r="AN101" s="55"/>
+      <c r="AO101" s="55"/>
+      <c r="AP101" s="55"/>
+      <c r="AQ101" s="55"/>
+      <c r="AR101" s="55"/>
+      <c r="AS101" s="55"/>
+      <c r="AT101" s="55"/>
+      <c r="AU101" s="55"/>
+      <c r="AV101" s="55"/>
+      <c r="AW101" s="55"/>
+      <c r="AX101" s="55"/>
+      <c r="AY101" s="55"/>
+      <c r="AZ101" s="55"/>
+      <c r="BA101" s="55"/>
+      <c r="BB101" s="55"/>
+      <c r="BC101" s="55"/>
+    </row>
+    <row r="102" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK102" s="55"/>
+      <c r="AL102" s="55"/>
+      <c r="AM102" s="55"/>
+      <c r="AN102" s="55"/>
+      <c r="AO102" s="55"/>
+      <c r="AP102" s="55"/>
+      <c r="AQ102" s="55"/>
+      <c r="AR102" s="55"/>
+      <c r="AS102" s="55"/>
+      <c r="AT102" s="55"/>
+      <c r="AU102" s="55"/>
+      <c r="AV102" s="55"/>
+      <c r="AW102" s="55"/>
+      <c r="AX102" s="55"/>
+      <c r="AY102" s="55"/>
+      <c r="AZ102" s="55"/>
+      <c r="BA102" s="55"/>
+      <c r="BB102" s="55"/>
+      <c r="BC102" s="55"/>
+    </row>
+    <row r="103" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK103" s="55"/>
+      <c r="AL103" s="55"/>
+      <c r="AM103" s="55"/>
+      <c r="AN103" s="55"/>
+      <c r="AO103" s="55"/>
+      <c r="AP103" s="55"/>
+      <c r="AQ103" s="55"/>
+      <c r="AR103" s="55"/>
+      <c r="AS103" s="55"/>
+      <c r="AT103" s="55"/>
+      <c r="AU103" s="55"/>
+      <c r="AV103" s="55"/>
+      <c r="AW103" s="55"/>
+      <c r="AX103" s="55"/>
+      <c r="AY103" s="55"/>
+      <c r="AZ103" s="55"/>
+      <c r="BA103" s="55"/>
+      <c r="BB103" s="55"/>
+      <c r="BC103" s="55"/>
+    </row>
+    <row r="104" spans="37:55" x14ac:dyDescent="0.3">
+      <c r="AK104" s="55"/>
+      <c r="AL104" s="55"/>
+      <c r="AM104" s="55"/>
+      <c r="AN104" s="55"/>
+      <c r="AO104" s="55"/>
+      <c r="AP104" s="55"/>
+      <c r="AQ104" s="55"/>
+      <c r="AR104" s="55"/>
+      <c r="AS104" s="55"/>
+      <c r="AT104" s="55"/>
+      <c r="AU104" s="55"/>
+      <c r="AV104" s="55"/>
+      <c r="AW104" s="55"/>
+      <c r="AX104" s="55"/>
+      <c r="AY104" s="55"/>
+      <c r="AZ104" s="55"/>
+      <c r="BA104" s="55"/>
+      <c r="BB104" s="55"/>
+      <c r="BC104" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4887,8 +5745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DD314E-C382-46AC-806D-7E5988604C2A}">
   <dimension ref="A1:AD297"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4921,14 +5779,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
       <c r="G1" s="11"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -4954,7 +5812,7 @@
       <c r="AC1" s="13"/>
       <c r="AD1" s="13"/>
     </row>
-    <row r="2" spans="1:30" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
@@ -5028,15 +5886,15 @@
         <v>131</v>
       </c>
       <c r="Y2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z2" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="8">
         <v>-5.3600000000000002E-3</v>
@@ -5116,7 +5974,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="8">
         <v>-2.988E-2</v>
@@ -5196,7 +6054,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="8">
         <v>-5.6349999999999997E-2</v>
@@ -5276,7 +6134,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="8">
         <v>-1.1780000000000001E-2</v>
@@ -5356,7 +6214,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" s="8">
         <v>1.828E-3</v>
@@ -5436,7 +6294,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="8">
         <v>-4.3869999999999998E-4</v>
@@ -5516,7 +6374,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="8">
         <v>-4.854E-2</v>
@@ -5596,7 +6454,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="8">
         <v>-5.0139999999999997E-2</v>
@@ -5676,7 +6534,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" s="8">
         <v>-0.1295</v>
@@ -5756,7 +6614,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="8">
         <v>-0.28889999999999999</v>
@@ -5836,7 +6694,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" s="8">
         <v>-0.16350000000000001</v>
@@ -5916,7 +6774,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" s="8">
         <v>-8.0399999999999999E-2</v>
@@ -5996,7 +6854,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" s="16">
         <v>0</v>
@@ -6076,7 +6934,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="16">
         <v>0</v>
@@ -6156,7 +7014,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="16">
         <v>0</v>
@@ -6236,7 +7094,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -6316,7 +7174,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="16">
         <v>0</v>
@@ -6396,7 +7254,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" s="16">
         <v>0</v>
@@ -6476,7 +7334,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21" s="16">
         <v>0</v>
@@ -6556,7 +7414,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19">
@@ -6623,7 +7481,7 @@
         <v>14000</v>
       </c>
       <c r="X22" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y22" s="20">
         <v>4.4000000000000004</v>
@@ -6634,7 +7492,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="24">
         <v>0</v>
@@ -6714,7 +7572,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24" s="24">
         <v>0</v>
@@ -6794,7 +7652,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B25" s="19">
         <v>1.7618</v>
@@ -6874,7 +7732,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B26" s="27">
         <v>1.268</v>
@@ -6954,7 +7812,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" s="8">
         <v>0.68540000000000001</v>
@@ -7034,7 +7892,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B28" s="8">
         <v>0.81169999999999998</v>
@@ -7114,7 +7972,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="8">
         <v>0.77680000000000005</v>
@@ -7194,7 +8052,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B30" s="8">
         <v>0.96760000000000002</v>
@@ -7274,7 +8132,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B31">
         <v>-3.3240000000000001E-3</v>
@@ -7354,7 +8212,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B32" s="8">
         <v>0.88239999999999996</v>
@@ -7434,7 +8292,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" s="8">
         <v>-4.854E-2</v>
@@ -7514,7 +8372,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B34">
         <v>1.2080000000000001E-3</v>
@@ -7594,7 +8452,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B35" s="35">
         <v>0</v>
@@ -7674,11 +8532,11 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="B36" s="53">
+        <v>169</v>
+      </c>
+      <c r="B36" s="52">
         <f>Y36</f>
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="C36" s="16">
         <v>0</v>
@@ -7740,22 +8598,22 @@
       <c r="V36" s="19">
         <v>0</v>
       </c>
-      <c r="W36" s="44">
+      <c r="W36" s="43">
         <v>5100</v>
       </c>
-      <c r="X36" s="45">
+      <c r="X36" s="44">
         <v>21</v>
       </c>
       <c r="Y36" s="10">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="Z36" s="8">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A37" s="54" t="s">
-        <v>162</v>
+      <c r="A37" s="53" t="s">
+        <v>161</v>
       </c>
       <c r="B37" s="8">
         <v>-5.0700000000000002E-2</v>
@@ -7820,10 +8678,10 @@
       <c r="V37" s="14">
         <v>-2.871E-8</v>
       </c>
-      <c r="W37" s="44">
+      <c r="W37" s="43">
         <v>5100</v>
       </c>
-      <c r="X37" s="45">
+      <c r="X37" s="44">
         <v>20</v>
       </c>
       <c r="Y37" s="34">
@@ -8646,6 +9504,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010026F0D136D79F25469E9BD90619CDB412" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4a869207c6945743f5de18208a2cfcba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f9188d7-3b18-4187-a3cb-7b6899b4ef8f" xmlns:ns3="85078965-a7f2-4dbb-adf6-2b7faeeb76ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89813893f4c0c91941f9d9d5434200cd" ns2:_="" ns3:_="">
     <xsd:import namespace="4f9188d7-3b18-4187-a3cb-7b6899b4ef8f"/>
@@ -8868,22 +9741,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BAFCAE4-A011-4769-B47E-67DBBC3AE6CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D6E2B2-1F78-45C8-93F5-31B8FF78EAA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51AA6EA-A3F6-4587-80EF-6E5C51392FC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8900,21 +9775,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BAFCAE4-A011-4769-B47E-67DBBC3AE6CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D6E2B2-1F78-45C8-93F5-31B8FF78EAA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>